<commit_message>
add digikey link for power headers
</commit_message>
<xml_diff>
--- a/VCO/Assembly/tht_bom.xlsx
+++ b/VCO/Assembly/tht_bom.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Designator</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>A-2939</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/68602-110HLF/2023310</t>
   </si>
   <si>
     <t>J8, J9</t>
@@ -180,6 +183,7 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -188,7 +192,6 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -248,11 +251,14 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
@@ -260,17 +266,14 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -576,106 +579,112 @@
       <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="7">
         <v>1.0</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="C6" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="E6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="14"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="C7" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="15" t="s">
+      <c r="E7" s="11" t="s">
         <v>31</v>
       </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="B8" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="11">
         <v>6.0</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>36</v>
       </c>
+      <c r="G8" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="14">
+      <c r="B9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="15">
         <v>1.0</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>40</v>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>41</v>
+      <c r="G9" s="18" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -711,7 +720,7 @@
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="15"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14">
@@ -9410,12 +9419,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="F8"/>
-    <hyperlink r:id="rId3" ref="G8"/>
-    <hyperlink r:id="rId4" ref="F9"/>
-    <hyperlink r:id="rId5" ref="G9"/>
+    <hyperlink r:id="rId2" ref="F4"/>
+    <hyperlink r:id="rId3" ref="F8"/>
+    <hyperlink r:id="rId4" ref="G8"/>
+    <hyperlink r:id="rId5" ref="F9"/>
+    <hyperlink r:id="rId6" ref="G9"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <drawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>